<commit_message>
Update of goodness of fit table
</commit_message>
<xml_diff>
--- a/figures and tables/2022 Figures and Tables/tables/TableS_OOS_gof_formatted.xlsx
+++ b/figures and tables/2022 Figures and Tables/tables/TableS_OOS_gof_formatted.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="TableS_OOS_gof" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>S-TS</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>RMSE (mg O2 m-2 d-1)</t>
+  </si>
+  <si>
+    <t>NRMSE</t>
   </si>
 </sst>
 </file>
@@ -548,7 +554,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -560,6 +566,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -884,47 +896,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:G12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="12.1796875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.08984375" customWidth="1"/>
+    <col min="6" max="11" width="12.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K1" s="5"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -933,237 +956,451 @@
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="6">
+        <v>3.3417383243704601</v>
+      </c>
+      <c r="C3" s="6">
+        <v>3.4333387307687002</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.22478478585283099</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.23094636277406999</v>
+      </c>
+      <c r="F3" s="2">
         <v>171.099145032536</v>
       </c>
-      <c r="C3" s="2">
+      <c r="G3" s="2">
         <v>160.483151399306</v>
       </c>
-      <c r="D3" s="2">
+      <c r="H3" s="2">
         <v>320.54747966311601</v>
       </c>
-      <c r="E3" s="2">
+      <c r="I3" s="2">
         <v>278.61831903531998</v>
       </c>
-      <c r="F3" s="2">
+      <c r="J3" s="2">
         <v>63.905325443787</v>
       </c>
-      <c r="G3" s="2">
+      <c r="K3" s="2">
         <v>69.526627218934905</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="6">
+        <v>1.1180404517792999</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.75129118862183897</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.22766261125606599</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.152982759741045</v>
+      </c>
+      <c r="F4" s="2">
         <v>138.46492015618199</v>
       </c>
-      <c r="C4" s="2">
+      <c r="G4" s="2">
         <v>91.6095639560438</v>
       </c>
-      <c r="D4" s="2">
+      <c r="H4" s="2">
         <v>592.36314779893098</v>
       </c>
-      <c r="E4" s="2">
+      <c r="I4" s="2">
         <v>363.24280371875699</v>
       </c>
-      <c r="F4" s="2">
+      <c r="J4" s="2">
         <v>90.822784810126606</v>
       </c>
-      <c r="G4" s="2">
+      <c r="K4" s="2">
         <v>89.240506329113899</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="6">
+        <v>1.1915197558550701</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1.1139766778684601</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.18653001002950301</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.174390797864967</v>
+      </c>
+      <c r="F5" s="2">
         <v>46.822787952059898</v>
       </c>
-      <c r="C5" s="2">
+      <c r="G5" s="2">
         <v>40.129563112785597</v>
       </c>
-      <c r="D5" s="2">
+      <c r="H5" s="2">
         <v>188.25033555543601</v>
       </c>
-      <c r="E5" s="2">
+      <c r="I5" s="2">
         <v>168.27278080352301</v>
       </c>
-      <c r="F5" s="2">
+      <c r="J5" s="2">
         <v>76.160990712074295</v>
       </c>
-      <c r="G5" s="2">
+      <c r="K5" s="2">
         <v>94.117647058823493</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="6">
+        <v>1.11699915242334</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1.02498398861837</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.311667980841285</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.28599367281011301</v>
+      </c>
+      <c r="F6" s="2">
         <v>18.768822834911301</v>
       </c>
-      <c r="C6" s="2">
+      <c r="G6" s="2">
         <v>27.926935394958299</v>
       </c>
-      <c r="D6" s="2">
+      <c r="H6" s="2">
         <v>80.636945095171399</v>
       </c>
-      <c r="E6" s="2">
+      <c r="I6" s="2">
         <v>75.063751039532406</v>
       </c>
-      <c r="F6" s="2">
+      <c r="J6" s="2">
         <v>86.416184971098303</v>
       </c>
-      <c r="G6" s="2">
+      <c r="K6" s="2">
         <v>93.930635838150295</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="6">
+        <v>4.1589269306042196</v>
+      </c>
+      <c r="C7" s="6">
+        <v>3.5121738846041399</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.26893364571336098</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.227111883167571</v>
+      </c>
+      <c r="F7" s="2">
         <v>5.6170952226388904</v>
       </c>
-      <c r="C7" s="2">
+      <c r="G7" s="2">
         <v>3.9118495687481101</v>
       </c>
-      <c r="D7" s="2">
+      <c r="H7" s="2">
         <v>26.769032272642601</v>
       </c>
-      <c r="E7" s="2">
+      <c r="I7" s="2">
         <v>6.87394562816639</v>
       </c>
-      <c r="F7" s="2">
+      <c r="J7" s="2">
         <v>96.735905044510403</v>
       </c>
-      <c r="G7" s="2">
+      <c r="K7" s="2">
         <v>89.317507418397597</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="6">
+        <v>2.1498946820767699</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1.84385684523717</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.22766871045582099</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.195260034698433</v>
+      </c>
+      <c r="F8" s="2">
         <v>696.31626523717398</v>
       </c>
-      <c r="C8" s="2">
+      <c r="G8" s="2">
         <v>855.94573143292996</v>
       </c>
-      <c r="D8" s="2">
+      <c r="H8" s="2">
         <v>573.18271658412095</v>
       </c>
-      <c r="E8" s="2">
+      <c r="I8" s="2">
         <v>690.34773169165703</v>
       </c>
-      <c r="F8" s="2">
+      <c r="J8" s="2">
         <v>80.141843971631204</v>
       </c>
-      <c r="G8" s="2">
+      <c r="K8" s="2">
         <v>85.106382978723403</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4">
-        <f>AVERAGE(B3:B8)</f>
+      <c r="B10" s="6">
+        <f t="shared" ref="B10:E10" si="0">AVERAGE(B3:B8)</f>
+        <v>2.1795198828515265</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9466035526197798</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.24120795735814451</v>
+      </c>
+      <c r="E10" s="6">
+        <f>AVERAGE(E3:E8)</f>
+        <v>0.21111425184269983</v>
+      </c>
+      <c r="F10" s="4">
+        <f>AVERAGE(F3:F8)</f>
         <v>179.514839405917</v>
       </c>
-      <c r="C10" s="4">
-        <f t="shared" ref="C10:G10" si="0">AVERAGE(C3:C8)</f>
+      <c r="G10" s="4">
+        <f t="shared" ref="G10:K10" si="1">AVERAGE(G3:G8)</f>
         <v>196.66779914412862</v>
       </c>
-      <c r="D10" s="4">
-        <f t="shared" si="0"/>
+      <c r="H10" s="4">
+        <f t="shared" si="1"/>
         <v>296.95827616156964</v>
       </c>
-      <c r="E10" s="4">
-        <f t="shared" si="0"/>
+      <c r="I10" s="4">
+        <f t="shared" si="1"/>
         <v>263.73655531949265</v>
       </c>
-      <c r="F10" s="4">
-        <f t="shared" si="0"/>
+      <c r="J10" s="4">
+        <f t="shared" si="1"/>
         <v>82.363839158871301</v>
       </c>
-      <c r="G10" s="4">
-        <f t="shared" si="0"/>
+      <c r="K10" s="4">
+        <f t="shared" si="1"/>
         <v>86.873217807023934</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4">
-        <f>MIN(B3:B8)</f>
+      <c r="B11" s="6">
+        <f t="shared" ref="B11:E11" si="2">MIN(B3:B8)</f>
+        <v>1.11699915242334</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="2"/>
+        <v>0.75129118862183897</v>
+      </c>
+      <c r="D11" s="6">
+        <f t="shared" si="2"/>
+        <v>0.18653001002950301</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="2"/>
+        <v>0.152982759741045</v>
+      </c>
+      <c r="F11" s="4">
+        <f>MIN(F3:F8)</f>
         <v>5.6170952226388904</v>
       </c>
-      <c r="C11" s="4">
-        <f t="shared" ref="C11:G11" si="1">MIN(C3:C8)</f>
+      <c r="G11" s="4">
+        <f t="shared" ref="G11:K11" si="3">MIN(G3:G8)</f>
         <v>3.9118495687481101</v>
       </c>
-      <c r="D11" s="4">
-        <f t="shared" si="1"/>
+      <c r="H11" s="4">
+        <f t="shared" si="3"/>
         <v>26.769032272642601</v>
       </c>
-      <c r="E11" s="4">
-        <f t="shared" si="1"/>
+      <c r="I11" s="4">
+        <f t="shared" si="3"/>
         <v>6.87394562816639</v>
       </c>
-      <c r="F11" s="4">
-        <f t="shared" si="1"/>
+      <c r="J11" s="4">
+        <f t="shared" si="3"/>
         <v>63.905325443787</v>
       </c>
-      <c r="G11" s="4">
-        <f t="shared" si="1"/>
+      <c r="K11" s="4">
+        <f t="shared" si="3"/>
         <v>69.526627218934905</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4">
-        <f>MAX(B3:B8)</f>
+      <c r="B12" s="6">
+        <f t="shared" ref="B12:E12" si="4">MAX(B3:B8)</f>
+        <v>4.1589269306042196</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" si="4"/>
+        <v>3.5121738846041399</v>
+      </c>
+      <c r="D12" s="6">
+        <f t="shared" si="4"/>
+        <v>0.311667980841285</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="4"/>
+        <v>0.28599367281011301</v>
+      </c>
+      <c r="F12" s="4">
+        <f>MAX(F3:F8)</f>
         <v>696.31626523717398</v>
       </c>
-      <c r="C12" s="4">
-        <f t="shared" ref="C12:G12" si="2">MAX(C3:C8)</f>
+      <c r="G12" s="4">
+        <f t="shared" ref="G12:K12" si="5">MAX(G3:G8)</f>
         <v>855.94573143292996</v>
       </c>
-      <c r="D12" s="4">
-        <f t="shared" si="2"/>
+      <c r="H12" s="4">
+        <f t="shared" si="5"/>
         <v>592.36314779893098</v>
       </c>
-      <c r="E12" s="4">
-        <f t="shared" si="2"/>
+      <c r="I12" s="4">
+        <f t="shared" si="5"/>
         <v>690.34773169165703</v>
       </c>
-      <c r="F12" s="4">
-        <f t="shared" si="2"/>
+      <c r="J12" s="4">
+        <f t="shared" si="5"/>
         <v>96.735905044510403</v>
       </c>
-      <c r="G12" s="4">
-        <f t="shared" si="2"/>
+      <c r="K12" s="4">
+        <f t="shared" si="5"/>
         <v>94.117647058823493</v>
       </c>
     </row>
+    <row r="21" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+    </row>
+    <row r="23" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+    </row>
+    <row r="24" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+    </row>
+    <row r="25" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+    </row>
+    <row r="26" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+    </row>
+    <row r="27" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+    </row>
+    <row r="28" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+    </row>
+    <row r="29" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+    </row>
+    <row r="30" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+    </row>
+    <row r="31" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+    </row>
+    <row r="32" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+    </row>
+    <row r="33" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="D1:E1"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>